<commit_message>
calculate depend on the open source data sets. And complete the writing of the report.
</commit_message>
<xml_diff>
--- a/Project/Project 2/Project_Carp/Project_Carp/CARPReportGradingRules.xlsx
+++ b/Project/Project 2/Project_Carp/Project_Carp/CARPReportGradingRules.xlsx
@@ -1,35 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhaoyao/Documents/AI/my/LAB2021/Lab/project-carp/Project_Carp/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B51F2D-5240-0B48-8E99-69060336A514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="3620" windowWidth="24240" windowHeight="11680" xr2:uid="{9106A175-1279-B942-BDC9-E3A3ED51A020}"/>
+    <workbookView windowWidth="10848" windowHeight="9275"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -37,7 +17,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>IMP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Items</t>
@@ -71,56 +50,9 @@
   </si>
   <si>
     <t>Problem Applications</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Methodology</t>
-  </si>
-  <si>
-    <t>3、Model design: how did you formulate the problem? How did you solve the problem? Descripe the main steps and the main algorithms you used in every step.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Empirical Verification</t>
-  </si>
-  <si>
-    <t>2.Performance measure:How did you measure the performance?How about you test envirment?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.Hyperparameters: How did you choose hyperparameters of your algorithms?(If you have no hyperparameters, you should discuss about parameters that can effect your performance and how to adjust them to get better performance)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.Experimental results (using table, figure, chart etc.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>References</t>
-  </si>
-  <si>
-    <t>List the references, please follow the IEEE format to prepare your references. The IEEE format can be found at:</t>
-  </si>
-  <si>
-    <t>http://ieeeauthorcenter.ieee.org/create-your-ieee-article/use-authoring-tools-and-ieee-article-templates/ieee-article-templates/templates-for-transactions/</t>
-  </si>
-  <si>
-    <t>(you can use google scholar to generate the above reference format). Note that any material (such as papers, slides, reports, etc.) you have cited in your report needs to be listed in the references.</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>4、Detail of algorithms: Descripe the function of the algorithms mentioned in Model design and write down their  pseudo-code. (Don't use any code picture, or pseudo-code picture, since we have no way of knowing whether you copied the pictures from somewhere or generated them yourself. If you did so, we will derectly take off 10 points.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. Conclusion:Analysis of the experimental results. (both advantages and disadvantages of your algorithms, summarize the experience you learned, deficiencies, and possible improvement directions in the future.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2、Data Structure:list all your key data structures. (For example, adj_list: a collection of lists represents graph)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Methodology 方法论</t>
   </si>
   <si>
     <r>
@@ -131,35 +63,79 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="DengXian"/>
-        <family val="4"/>
         <charset val="134"/>
       </rPr>
-      <t>)</t>
+      <t>)列举出所有用到的符号，例如</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Dataset: Which data did you use?(Except for the data that carp platform supply)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Q：车辆容量。</t>
+    </r>
+  </si>
+  <si>
+    <t>2、Data Structure:list all your key data structures. (For example, adj_list: a collection of lists represents graph)列举出所有使用到的关键数据结构。</t>
+  </si>
+  <si>
+    <t>3、Model design: how did you formulate the problem? How did you solve the problem? Descripe the main steps and the main algorithms you used in every step.模型设计：你是如何阐述这个问题的，你是如何解决这个问题的，描述解决这个问题的主要步骤和每个步骤中使用的算法。</t>
+  </si>
+  <si>
+    <t>4、Detail of algorithms: Descripe the function of the algorithms mentioned in Model design and write down their  pseudo-code. (Don't use any code picture, or pseudo-code picture, since we have no way of knowing whether you copied the pictures from somewhere or generated them yourself. If you did so, we will derectly take off 10 points.)算法细节，描述前面模型设计中提及的算法，并写下它们的伪代码。</t>
+  </si>
+  <si>
+    <t>Empirical Verification 经验验证</t>
+  </si>
+  <si>
+    <t>1. Dataset: Which data did you use?(Except for the data that carp platform supply)数据集的使用，除了平台提供的数据集，还使用了哪些数据？</t>
+  </si>
+  <si>
+    <t>2.Performance measure:How did you measure the performance?How about you test envirment?绩效评估，你的测试结果如何？你用什么来评估你的表现的？你的测试环境是什么？</t>
+  </si>
+  <si>
+    <t>3.Hyperparameters: How did you choose hyperparameters of your algorithms?(If you have no hyperparameters, you should discuss about parameters that can effect your performance and how to adjust them to get better performance)超参数：你是如何选择算法中的超参数的？</t>
+  </si>
+  <si>
+    <t>4.Experimental results (using table, figure, chart etc.) 实验结果</t>
+  </si>
+  <si>
+    <t>5. Conclusion:Analysis of the experimental results. (both advantages and disadvantages of your algorithms, summarize the experience you learned, deficiencies, and possible improvement directions in the future.)结论：分析实验结果，包括算法的优势和劣势，总结实验中学到的内容，缺陷，和可能的未来的改进方向。</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>List the references, please follow the IEEE format to prepare your references. The IEEE format can be found at:列出参考文献</t>
+  </si>
+  <si>
+    <t>http://ieeeauthorcenter.ieee.org/create-your-ieee-article/use-authoring-tools-and-ieee-article-templates/ieee-article-templates/templates-for-transactions/</t>
+  </si>
+  <si>
+    <t>(you can use google scholar to generate the above reference format). Note that any material (such as papers, slides, reports, etc.) you have cited in your report needs to be listed in the references.</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -167,27 +143,362 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="DengXian"/>
-      <family val="4"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -280,48 +591,334 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -370,7 +967,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -403,26 +1000,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -455,23 +1035,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -613,27 +1176,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E20D3ADD-EF90-1142-A230-331D4053E60F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="69.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="69.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -733,170 +1291,170 @@
       <c r="F7" s="5"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="34">
+    <row r="8" ht="31.2" spans="1:7">
       <c r="A8" s="1"/>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="C8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6">
         <v>10</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="34">
+    <row r="9" ht="31.2" spans="1:7">
       <c r="A9" s="1"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="6" t="s">
-        <v>25</v>
+      <c r="B9" s="8"/>
+      <c r="C9" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="D9" s="8">
         <v>10</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="51">
+    <row r="10" ht="62.4" spans="1:7">
       <c r="A10" s="1"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="6" t="s">
-        <v>13</v>
+      <c r="B10" s="8"/>
+      <c r="C10" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="D10" s="8">
         <v>10</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="85">
+    <row r="11" ht="78" spans="1:7">
       <c r="A11" s="1"/>
-      <c r="B11" s="14"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D11" s="4">
         <v>10</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="34">
+    <row r="12" ht="31.2" spans="1:7">
       <c r="A12" s="1"/>
-      <c r="B12" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="6">
         <v>6</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="34">
+    <row r="13" ht="46.8" spans="1:7">
       <c r="A13" s="1"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="6" t="s">
-        <v>15</v>
+      <c r="B13" s="8"/>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="8">
         <v>6</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="68">
+    <row r="14" ht="62.4" spans="1:7">
       <c r="A14" s="1"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="6" t="s">
-        <v>16</v>
+      <c r="B14" s="8"/>
+      <c r="C14" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="D14" s="8">
         <v>6</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" ht="17">
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="6" t="s">
-        <v>17</v>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="D15" s="8">
         <v>6</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="51">
+    <row r="16" ht="62.4" spans="1:7">
       <c r="A16" s="1"/>
-      <c r="B16" s="14"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" s="4">
         <v>6</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="34">
+    <row r="17" ht="31.2" spans="1:7">
       <c r="A17" s="1"/>
-      <c r="B17" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="12">
+      <c r="B17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="6">
         <v>5</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="51">
+    <row r="18" ht="27.6" spans="1:7">
       <c r="A18" s="1"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" ht="51">
+    <row r="19" ht="46.8" spans="1:7">
       <c r="A19" s="1"/>
-      <c r="B19" s="14"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="10" t="s">
-        <v>22</v>
+      <c r="D20" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -913,18 +1471,21 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B16"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E16"/>
     <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="F12:F16"/>
     <mergeCell ref="F17:F19"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="F12:F16"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C18" r:id="rId1" display="http://ieeeauthorcenter.ieee.org/create-your-ieee-article/use-authoring-tools-and-ieee-article-templates/ieee-article-templates/templates-for-transactions/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update the report, however, there are something wrong on the formatting.
</commit_message>
<xml_diff>
--- a/Project/Project 2/Project_Carp/Project_Carp/CARPReportGradingRules.xlsx
+++ b/Project/Project 2/Project_Carp/Project_Carp/CARPReportGradingRules.xlsx
@@ -56,6 +56,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>1、Notation: list all your notations used in your report. (For example, Q:Vehicle capacity</t>
     </r>
     <r>
@@ -126,10 +133,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -158,78 +165,70 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -268,15 +267,23 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -285,14 +292,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -313,187 +320,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,17 +596,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -618,15 +614,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -642,6 +629,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -657,24 +662,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -689,51 +676,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -745,97 +755,94 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1184,8 +1191,8 @@
   <sheetPr/>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="6"/>

</xml_diff>